<commit_message>
aanpassing documentatie op basis van besluit objecttoestand
</commit_message>
<xml_diff>
--- a/tabellen/actueel/5.02_hoofdgroepen.xlsx
+++ b/tabellen/actueel/5.02_hoofdgroepen.xlsx
@@ -1,20 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\100289\OneDrive\GitHub\NLCS\tabellen\ontwikkeling\versie-5.0-LinkedData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\100289\OneDrive\GitHub\NLCS\tabellen\actueel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{98D20513-141F-4575-A23B-B946E83461DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EC02430-BAD8-42C5-AC17-3B414EDA6B6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="5.01_hoofdgroepen" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'5.01_hoofdgroepen'!$A$1:$D$33</definedName>
+  </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
@@ -325,7 +328,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -864,9 +867,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Thema">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -904,7 +907,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1010,7 +1013,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1152,21 +1155,25 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="71.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.08984375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
@@ -1184,453 +1191,458 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>37</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>5</v>
+        <v>38</v>
       </c>
       <c r="D2" t="s">
-        <v>6</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>70</v>
       </c>
       <c r="B3">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>8</v>
+        <v>71</v>
       </c>
       <c r="D3" t="s">
-        <v>9</v>
+        <v>72</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>82</v>
       </c>
       <c r="B4">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>11</v>
+        <v>83</v>
       </c>
       <c r="D4" t="s">
-        <v>12</v>
+        <v>84</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>43</v>
       </c>
       <c r="B5">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="C5" t="s">
-        <v>14</v>
+        <v>44</v>
       </c>
       <c r="D5" t="s">
-        <v>15</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>16</v>
+        <v>85</v>
       </c>
       <c r="B6">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>17</v>
+        <v>86</v>
       </c>
       <c r="D6" t="s">
-        <v>18</v>
+        <v>87</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>19</v>
+        <v>46</v>
       </c>
       <c r="B7">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="C7" t="s">
-        <v>20</v>
+        <v>47</v>
       </c>
       <c r="D7" t="s">
-        <v>21</v>
+        <v>48</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>22</v>
+        <v>91</v>
       </c>
       <c r="B8">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>23</v>
+        <v>92</v>
       </c>
       <c r="D8" t="s">
-        <v>24</v>
+        <v>93</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>25</v>
+        <v>49</v>
       </c>
       <c r="B9">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="C9" t="s">
-        <v>26</v>
+        <v>50</v>
       </c>
       <c r="D9" t="s">
-        <v>27</v>
+        <v>51</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>28</v>
+        <v>88</v>
       </c>
       <c r="B10">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="C10" t="s">
-        <v>29</v>
+        <v>89</v>
       </c>
       <c r="D10" t="s">
-        <v>30</v>
+        <v>90</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>31</v>
+        <v>94</v>
       </c>
       <c r="B11">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="C11" t="s">
-        <v>32</v>
+        <v>95</v>
       </c>
       <c r="D11" t="s">
-        <v>33</v>
+        <v>96</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>34</v>
+        <v>52</v>
       </c>
       <c r="B12">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="C12" t="s">
-        <v>35</v>
+        <v>53</v>
       </c>
       <c r="D12" t="s">
-        <v>36</v>
+        <v>54</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>37</v>
+        <v>55</v>
       </c>
       <c r="B13">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="C13" t="s">
-        <v>38</v>
+        <v>56</v>
       </c>
       <c r="D13" t="s">
-        <v>39</v>
+        <v>57</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>40</v>
+        <v>97</v>
       </c>
       <c r="B14">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="C14" t="s">
-        <v>41</v>
+        <v>98</v>
       </c>
       <c r="D14" t="s">
-        <v>42</v>
+        <v>99</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>43</v>
+        <v>76</v>
       </c>
       <c r="B15">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="C15" t="s">
-        <v>44</v>
+        <v>77</v>
       </c>
       <c r="D15" t="s">
-        <v>45</v>
+        <v>78</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>46</v>
+        <v>73</v>
       </c>
       <c r="B16">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="C16" t="s">
-        <v>47</v>
+        <v>74</v>
       </c>
       <c r="D16" t="s">
-        <v>48</v>
+        <v>75</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>49</v>
+        <v>10</v>
       </c>
       <c r="B17">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="C17" t="s">
-        <v>50</v>
+        <v>11</v>
       </c>
       <c r="D17" t="s">
-        <v>51</v>
+        <v>12</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>52</v>
+        <v>7</v>
       </c>
       <c r="B18">
-        <v>24</v>
+        <v>10</v>
       </c>
       <c r="C18" t="s">
-        <v>53</v>
+        <v>8</v>
       </c>
       <c r="D18" t="s">
-        <v>54</v>
+        <v>9</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="B19">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="C19" t="s">
-        <v>56</v>
+        <v>65</v>
       </c>
       <c r="D19" t="s">
-        <v>57</v>
+        <v>66</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>58</v>
+        <v>13</v>
       </c>
       <c r="B20">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="C20" t="s">
-        <v>59</v>
+        <v>14</v>
       </c>
       <c r="D20" t="s">
-        <v>60</v>
+        <v>15</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B21">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C21" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D21" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="B22">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C22" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="D22" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>67</v>
+        <v>16</v>
       </c>
       <c r="B23">
-        <v>29</v>
+        <v>13</v>
       </c>
       <c r="C23" t="s">
-        <v>68</v>
+        <v>17</v>
       </c>
       <c r="D23" t="s">
-        <v>69</v>
+        <v>18</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>70</v>
+        <v>19</v>
       </c>
       <c r="B24">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="C24" t="s">
-        <v>71</v>
+        <v>20</v>
       </c>
       <c r="D24" t="s">
-        <v>72</v>
+        <v>21</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>73</v>
+        <v>22</v>
       </c>
       <c r="B25">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="C25" t="s">
-        <v>74</v>
+        <v>23</v>
       </c>
       <c r="D25" t="s">
-        <v>75</v>
+        <v>24</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="B26">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C26" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="D26" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>79</v>
+        <v>25</v>
       </c>
       <c r="B27">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="C27" t="s">
-        <v>80</v>
+        <v>26</v>
       </c>
       <c r="D27" t="s">
-        <v>81</v>
+        <v>27</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>82</v>
+        <v>61</v>
       </c>
       <c r="B28">
-        <v>4</v>
+        <v>27</v>
       </c>
       <c r="C28" t="s">
-        <v>83</v>
+        <v>62</v>
       </c>
       <c r="D28" t="s">
-        <v>84</v>
+        <v>63</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>85</v>
+        <v>28</v>
       </c>
       <c r="B29">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="C29" t="s">
-        <v>86</v>
+        <v>29</v>
       </c>
       <c r="D29" t="s">
-        <v>87</v>
+        <v>30</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>88</v>
+        <v>31</v>
       </c>
       <c r="B30">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="C30" t="s">
-        <v>89</v>
+        <v>32</v>
       </c>
       <c r="D30" t="s">
-        <v>90</v>
+        <v>33</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>91</v>
+        <v>34</v>
       </c>
       <c r="B31">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="C31" t="s">
-        <v>92</v>
+        <v>35</v>
       </c>
       <c r="D31" t="s">
-        <v>93</v>
+        <v>36</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>94</v>
+        <v>4</v>
       </c>
       <c r="B32">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="C32" t="s">
-        <v>95</v>
+        <v>5</v>
       </c>
       <c r="D32" t="s">
-        <v>96</v>
+        <v>6</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>97</v>
+        <v>40</v>
       </c>
       <c r="B33">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="C33" t="s">
-        <v>98</v>
+        <v>41</v>
       </c>
       <c r="D33" t="s">
-        <v>99</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:D33" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D33">
+      <sortCondition ref="C1:C33"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>